<commit_message>
Export Xelpmoc Investments as html for online viewing
</commit_message>
<xml_diff>
--- a/ind/Xelpmoc/Xelpmoc Investments.xlsx
+++ b/ind/Xelpmoc/Xelpmoc Investments.xlsx
@@ -19,33 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13" count="13">
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Sector</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4" count="4">
   <si>
     <t>Percent</t>
-  </si>
-  <si>
-    <t>Investment Cost</t>
-  </si>
-  <si>
-    <t>March 2021 Value</t>
-  </si>
-  <si>
-    <t>March 2020 Value</t>
-  </si>
-  <si>
-    <t>March 2019 Value</t>
-  </si>
-  <si>
-    <t>March 2018 Value</t>
-  </si>
-  <si>
-    <t>Remarks</t>
   </si>
   <si>
     <t>Social networking</t>
@@ -55,9 +31,6 @@
   </si>
   <si>
     <t>Edutech</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -115,12 +88,15 @@
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="1" fillId="0" borderId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="right" vertical="justify" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -134,14 +110,14 @@
   <dimension ref="A1:IV32"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A1" sqref="A1:IV1 A2:IV2"/>
+      <selection activeCell="C2" sqref="C2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" style="0" width="24.569951923076925" customWidth="1"/>
     <col min="2" max="2" style="0" width="25.9984375" customWidth="1"/>
-    <col min="3" max="256" style="0" width="9.142307692307693"/>
+    <col min="3" max="16384" style="0" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:256">
@@ -151,33 +127,49 @@
         </is>
       </c>
     </row>
-    <row r="2" spans="1:256">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:256" ht="34.5">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Sector</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>8</v>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Investment Cost</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>March 2021 Value</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>March 2020 Value</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>March 2019 Value</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>March 2018 Value</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>Remarks</t>
+        </is>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -494,7 +486,7 @@
         </is>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>13.699999999999999</v>
@@ -509,10 +501,10 @@
         <v>37.5</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:256">
@@ -542,7 +534,7 @@
         <v>37.899999999999999</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:256">
@@ -569,10 +561,10 @@
         <v>4.5</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:256">
@@ -632,7 +624,7 @@
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:256">
@@ -642,7 +634,7 @@
         </is>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -651,13 +643,13 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:256">
@@ -706,13 +698,13 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -738,13 +730,13 @@
         <v>2.1000000000000001</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:256">
@@ -784,7 +776,7 @@
         </is>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>9.9000000000000004</v>
@@ -796,7 +788,7 @@
         <v>0.29999999999999999</v>
       </c>
       <c r="H15" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -849,10 +841,10 @@
         <v>2.5</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G17">
         <v>2.7000000000000002</v>
@@ -871,13 +863,13 @@
         <v>0.02</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H18">
         <v>0.014999999999999999</v>
@@ -893,16 +885,16 @@
         <v>1.25</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G19">
         <v>1.25</v>
       </c>
       <c r="H19" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:256">
@@ -921,10 +913,10 @@
         <v>0.40000000000000002</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H20" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -942,16 +934,16 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H21" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:256">
@@ -964,10 +956,10 @@
         <v>0.029999999999999999</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G22">
         <v>2.7000000000000002</v>
@@ -994,16 +986,16 @@
         <v>0.27000000000000002</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H23" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1029,7 +1021,7 @@
         <v>0.23999999999999999</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1055,7 +1047,7 @@
         <v>2.5</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1081,7 +1073,7 @@
         <v>1.77</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1096,7 +1088,7 @@
         </is>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -1105,16 +1097,16 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1140,16 +1132,16 @@
         <v>0.16</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H28" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -1158,8 +1150,10 @@
       </c>
     </row>
     <row r="32" spans="1:256">
-      <c r="A32" t="s">
-        <v>12</v>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
       </c>
       <c r="D32">
         <f>SUM(D3:D30)</f>

</xml_diff>